<commit_message>
Initial change made to sample data
</commit_message>
<xml_diff>
--- a/BusinessRulesExcelMockup.xlsx
+++ b/BusinessRulesExcelMockup.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="302">
   <si>
     <t>R3</t>
   </si>
@@ -1624,6 +1624,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test </t>
+  </si>
+  <si>
+    <t>Hello everyone! This is a GitHub Desktop Demonstration</t>
   </si>
 </sst>
 </file>
@@ -2131,6 +2134,72 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2139,72 +2208,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2650,10 +2653,13 @@
   <dimension ref="A1:AU64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="B63" sqref="B63:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
@@ -2669,22 +2675,22 @@
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="76" t="s">
+      <c r="L1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="77"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="79" t="s">
+      <c r="M1" s="70"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="79"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="79"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="72"/>
       <c r="X1" s="7" t="s">
         <v>3</v>
       </c>
@@ -2694,33 +2700,33 @@
       <c r="Z1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="81" t="s">
+      <c r="AA1" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="79" t="s">
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="80"/>
-      <c r="AF1" s="80"/>
-      <c r="AG1" s="80"/>
-      <c r="AH1" s="80"/>
-      <c r="AI1" s="81" t="s">
+      <c r="AE1" s="73"/>
+      <c r="AF1" s="73"/>
+      <c r="AG1" s="73"/>
+      <c r="AH1" s="73"/>
+      <c r="AI1" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="AJ1" s="82"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="82"/>
-      <c r="AM1" s="82"/>
-      <c r="AN1" s="67" t="s">
+      <c r="AJ1" s="75"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="75"/>
+      <c r="AM1" s="75"/>
+      <c r="AN1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="69"/>
+      <c r="AO1" s="59"/>
+      <c r="AP1" s="59"/>
+      <c r="AQ1" s="59"/>
+      <c r="AR1" s="59"/>
+      <c r="AS1" s="60"/>
       <c r="AT1" s="10" t="s">
         <v>10</v>
       </c>
@@ -3926,38 +3932,38 @@
       <c r="AU18" s="40"/>
     </row>
     <row r="19" spans="1:47" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64" t="s">
+      <c r="D19" s="65"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="J19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="63" t="s">
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="M19" s="63" t="s">
+      <c r="M19" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="N19" s="66" t="s">
+      <c r="N19" s="78" t="s">
         <v>120</v>
       </c>
       <c r="O19" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="P19" s="66" t="s">
+      <c r="P19" s="78" t="s">
         <v>121</v>
       </c>
       <c r="Q19" s="37" t="s">
@@ -3967,64 +3973,64 @@
         <v>123</v>
       </c>
       <c r="S19" s="37"/>
-      <c r="T19" s="63" t="s">
+      <c r="T19" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="U19" s="63" t="s">
+      <c r="U19" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="V19" s="63"/>
-      <c r="W19" s="63"/>
-      <c r="X19" s="63"/>
-      <c r="Y19" s="63"/>
+      <c r="V19" s="76"/>
+      <c r="W19" s="76"/>
+      <c r="X19" s="76"/>
+      <c r="Y19" s="76"/>
       <c r="Z19" s="29"/>
-      <c r="AA19" s="62"/>
-      <c r="AB19" s="62"/>
-      <c r="AC19" s="62" t="s">
+      <c r="AA19" s="79"/>
+      <c r="AB19" s="79"/>
+      <c r="AC19" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="63"/>
-      <c r="AE19" s="63"/>
-      <c r="AF19" s="63"/>
-      <c r="AG19" s="63"/>
-      <c r="AH19" s="63"/>
-      <c r="AI19" s="62">
+      <c r="AD19" s="76"/>
+      <c r="AE19" s="76"/>
+      <c r="AF19" s="76"/>
+      <c r="AG19" s="76"/>
+      <c r="AH19" s="76"/>
+      <c r="AI19" s="79">
         <v>1</v>
       </c>
-      <c r="AJ19" s="62"/>
-      <c r="AK19" s="62"/>
-      <c r="AL19" s="62"/>
-      <c r="AM19" s="62"/>
-      <c r="AN19" s="58"/>
-      <c r="AO19" s="58"/>
-      <c r="AP19" s="58"/>
-      <c r="AQ19" s="58"/>
-      <c r="AR19" s="58"/>
-      <c r="AS19" s="58"/>
-      <c r="AT19" s="60" t="s">
+      <c r="AJ19" s="79"/>
+      <c r="AK19" s="79"/>
+      <c r="AL19" s="79"/>
+      <c r="AM19" s="79"/>
+      <c r="AN19" s="80"/>
+      <c r="AO19" s="80"/>
+      <c r="AP19" s="80"/>
+      <c r="AQ19" s="80"/>
+      <c r="AR19" s="80"/>
+      <c r="AS19" s="80"/>
+      <c r="AT19" s="82" t="s">
         <v>126</v>
       </c>
       <c r="AU19" s="42"/>
     </row>
     <row r="20" spans="1:47" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="61"/>
-      <c r="N20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
       <c r="O20" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="P20" s="61"/>
+      <c r="P20" s="62"/>
       <c r="Q20" s="37" t="s">
         <v>127</v>
       </c>
@@ -4032,33 +4038,33 @@
         <v>128</v>
       </c>
       <c r="S20" s="37"/>
-      <c r="T20" s="61"/>
-      <c r="U20" s="61"/>
-      <c r="V20" s="61"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
-      <c r="Y20" s="61"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="62"/>
+      <c r="V20" s="62"/>
+      <c r="W20" s="62"/>
+      <c r="X20" s="62"/>
+      <c r="Y20" s="62"/>
       <c r="Z20" s="29"/>
-      <c r="AA20" s="61"/>
-      <c r="AB20" s="61"/>
-      <c r="AC20" s="61"/>
-      <c r="AD20" s="61"/>
-      <c r="AE20" s="61"/>
-      <c r="AF20" s="61"/>
-      <c r="AG20" s="61"/>
-      <c r="AH20" s="61"/>
-      <c r="AI20" s="61"/>
-      <c r="AJ20" s="61"/>
-      <c r="AK20" s="61"/>
-      <c r="AL20" s="61"/>
-      <c r="AM20" s="61"/>
-      <c r="AN20" s="59"/>
-      <c r="AO20" s="59"/>
-      <c r="AP20" s="59"/>
-      <c r="AQ20" s="59"/>
-      <c r="AR20" s="59"/>
-      <c r="AS20" s="59"/>
-      <c r="AT20" s="61"/>
+      <c r="AA20" s="62"/>
+      <c r="AB20" s="62"/>
+      <c r="AC20" s="62"/>
+      <c r="AD20" s="62"/>
+      <c r="AE20" s="62"/>
+      <c r="AF20" s="62"/>
+      <c r="AG20" s="62"/>
+      <c r="AH20" s="62"/>
+      <c r="AI20" s="62"/>
+      <c r="AJ20" s="62"/>
+      <c r="AK20" s="62"/>
+      <c r="AL20" s="62"/>
+      <c r="AM20" s="62"/>
+      <c r="AN20" s="81"/>
+      <c r="AO20" s="81"/>
+      <c r="AP20" s="81"/>
+      <c r="AQ20" s="81"/>
+      <c r="AR20" s="81"/>
+      <c r="AS20" s="81"/>
+      <c r="AT20" s="62"/>
       <c r="AU20" s="43"/>
     </row>
     <row r="21" spans="1:47" ht="96" x14ac:dyDescent="0.25">
@@ -6496,8 +6502,10 @@
         <v>299</v>
       </c>
     </row>
-    <row r="63" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A63" s="57"/>
+    <row r="63" spans="1:47" ht="24" x14ac:dyDescent="0.25">
+      <c r="A63" s="57" t="s">
+        <v>301</v>
+      </c>
       <c r="B63" s="57"/>
       <c r="C63" s="57"/>
     </row>
@@ -6506,6 +6514,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="AS19:AS20"/>
+    <mergeCell ref="AT19:AT20"/>
+    <mergeCell ref="AM19:AM20"/>
+    <mergeCell ref="AN19:AN20"/>
+    <mergeCell ref="AO19:AO20"/>
+    <mergeCell ref="AP19:AP20"/>
+    <mergeCell ref="AQ19:AQ20"/>
+    <mergeCell ref="AR19:AR20"/>
+    <mergeCell ref="AL19:AL20"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="AD19:AD20"/>
+    <mergeCell ref="AE19:AE20"/>
+    <mergeCell ref="AF19:AF20"/>
+    <mergeCell ref="AG19:AG20"/>
+    <mergeCell ref="AH19:AH20"/>
+    <mergeCell ref="AI19:AI20"/>
+    <mergeCell ref="AJ19:AJ20"/>
+    <mergeCell ref="AK19:AK20"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="X19:X20"/>
     <mergeCell ref="AN1:AS1"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
@@ -6522,38 +6562,6 @@
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="AD1:AH1"/>
     <mergeCell ref="AI1:AM1"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="AL19:AL20"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AD19:AD20"/>
-    <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="AF19:AF20"/>
-    <mergeCell ref="AG19:AG20"/>
-    <mergeCell ref="AH19:AH20"/>
-    <mergeCell ref="AI19:AI20"/>
-    <mergeCell ref="AJ19:AJ20"/>
-    <mergeCell ref="AK19:AK20"/>
-    <mergeCell ref="AS19:AS20"/>
-    <mergeCell ref="AT19:AT20"/>
-    <mergeCell ref="AM19:AM20"/>
-    <mergeCell ref="AN19:AN20"/>
-    <mergeCell ref="AO19:AO20"/>
-    <mergeCell ref="AP19:AP20"/>
-    <mergeCell ref="AQ19:AQ20"/>
-    <mergeCell ref="AR19:AR20"/>
   </mergeCells>
   <conditionalFormatting sqref="B1 B3:B18 B21:B51">
     <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="yesterday">
@@ -6654,7 +6662,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9B94903-ABCB-404E-81F7-82DF80C59736}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72452A5B-347A-4AF6-B010-6DA62BE29684}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>